<commit_message>
Cambios en la función. Se añadió la función invarianza a "0-funciones-nuevas" y se hicieron cambios en "1-cfa.y-reporte"
</commit_message>
<xml_diff>
--- a/Bases ejemplo/MIAU2021.xlsx
+++ b/Bases ejemplo/MIAU2021.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\UMC\Github\UMC\Bases ejemplo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F78A65-6617-444F-8F02-533F2CD5B447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="MFinal 2P, 4P, 6P, 2S" sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
     <definedName name="Z_E02B9B3C_46F0_4728_91B3_E7CBF51265FB_.wvu.FilterData" localSheetId="0" hidden="1">'MFinal 2P, 4P, 6P, 2S'!$A$1:$AH$34</definedName>
     <definedName name="Z_FCCC49F7_5622_4BA0_827A_A37B5870D922_.wvu.FilterData" localSheetId="0" hidden="1">'MFinal 2P, 4P, 6P, 2S'!$A$1:$AH$34</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <customWorkbookViews>
     <customWorkbookView name="Filtro Victor" guid="{61937B1B-5A62-4630-A349-DBF2AAB653FC}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Estefanía" guid="{E02B9B3C-46F0-4728-91B3-E7CBF51265FB}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
@@ -47,12 +46,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="165">
   <si>
     <t>EV</t>
   </si>
@@ -500,13 +499,85 @@
   </si>
   <si>
     <t>Antes de criticar a alguien, trato de imaginarme cómo me sentiría yo si estuviera en su lugar</t>
+  </si>
+  <si>
+    <t>EVA2021_2Sestudiante_EBRG1</t>
+  </si>
+  <si>
+    <t>p10</t>
+  </si>
+  <si>
+    <t>p10_01</t>
+  </si>
+  <si>
+    <t>¿Qué tan de acuerdo o en desacuerdo estás con los siguientes enunciados sobre tus padres o cuidadores principales?</t>
+  </si>
+  <si>
+    <t>Cuando mis padres quieren que haga algo, me explican por qué quieren que lo haga.</t>
+  </si>
+  <si>
+    <t>EST2SGEN_APFAUT</t>
+  </si>
+  <si>
+    <t>Apoyo a la autonomía</t>
+  </si>
+  <si>
+    <t>p10_02</t>
+  </si>
+  <si>
+    <t>Mi punto de vista es importante cuando mis padres toman decisiones que me involucran.</t>
+  </si>
+  <si>
+    <t>p10_03</t>
+  </si>
+  <si>
+    <t>Cuando mis padres me prohiben hacer algo, me explican por qué.</t>
+  </si>
+  <si>
+    <t>p10_04</t>
+  </si>
+  <si>
+    <t>Mis padres son capaces de ponerse en mi lugar y entender lo que siento.</t>
+  </si>
+  <si>
+    <t>p10_05</t>
+  </si>
+  <si>
+    <t>Mis padres esperan que tome decisiones que correspondan con mis intereses, independientemente de lo que ellos quieran para mí.</t>
+  </si>
+  <si>
+    <t>p10_06</t>
+  </si>
+  <si>
+    <t>Mis padres están abiertos a mi forma de pensar y sentir.</t>
+  </si>
+  <si>
+    <t>p10_07</t>
+  </si>
+  <si>
+    <t>Mis padres se aseguran de qué entienda por qué a veces me prohíben algunas cosas.</t>
+  </si>
+  <si>
+    <t>p10_08</t>
+  </si>
+  <si>
+    <t>Cuando pregunto a mis padres por qué no debo hacer algo, siempre me explican las razones.</t>
+  </si>
+  <si>
+    <t>p10_09</t>
+  </si>
+  <si>
+    <t>Cuando mis padres y yo no estamos de acuerdo en algo, siempre escuchan mi punto de vista.</t>
+  </si>
+  <si>
+    <t>Factor asociado al aprendizaje autorregulado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -549,8 +620,21 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -569,8 +653,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -593,11 +689,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -628,20 +799,47 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -851,18 +1049,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AH34"/>
+  <dimension ref="A1:AH43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="9.85546875" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" customWidth="1"/>
@@ -888,7 +1086,7 @@
     <col min="29" max="29" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" ht="12.75">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -992,7 +1190,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" ht="12.75">
       <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
@@ -1071,7 +1269,7 @@
       <c r="AG2" s="9"/>
       <c r="AH2" s="2"/>
     </row>
-    <row r="3" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" ht="12.75">
       <c r="A3" s="6" t="s">
         <v>34</v>
       </c>
@@ -1150,7 +1348,7 @@
       <c r="AG3" s="9"/>
       <c r="AH3" s="2"/>
     </row>
-    <row r="4" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" ht="12.75">
       <c r="A4" s="6" t="s">
         <v>34</v>
       </c>
@@ -1229,7 +1427,7 @@
       <c r="AG4" s="9"/>
       <c r="AH4" s="2"/>
     </row>
-    <row r="5" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" ht="18" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>34</v>
       </c>
@@ -1308,7 +1506,7 @@
       <c r="AG5" s="9"/>
       <c r="AH5" s="2"/>
     </row>
-    <row r="6" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" ht="19.5" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
@@ -1371,8 +1569,12 @@
         <v>46</v>
       </c>
       <c r="Y6" s="9"/>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="12"/>
+      <c r="Z6" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA6" s="12" t="s">
+        <v>48</v>
+      </c>
       <c r="AB6" s="10" t="s">
         <v>49</v>
       </c>
@@ -1385,7 +1587,7 @@
       <c r="AG6" s="9"/>
       <c r="AH6" s="2"/>
     </row>
-    <row r="7" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" ht="12.75">
       <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
@@ -1466,7 +1668,7 @@
       <c r="AG7" s="9"/>
       <c r="AH7" s="2"/>
     </row>
-    <row r="8" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" ht="15.75" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
@@ -1545,7 +1747,7 @@
       <c r="AG8" s="9"/>
       <c r="AH8" s="2"/>
     </row>
-    <row r="9" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" ht="12.75">
       <c r="A9" s="6" t="s">
         <v>34</v>
       </c>
@@ -1624,7 +1826,7 @@
       <c r="AG9" s="9"/>
       <c r="AH9" s="2"/>
     </row>
-    <row r="10" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" ht="12.75">
       <c r="A10" s="6" t="s">
         <v>34</v>
       </c>
@@ -1703,7 +1905,7 @@
       <c r="AG10" s="9"/>
       <c r="AH10" s="2"/>
     </row>
-    <row r="11" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" ht="12.75">
       <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
@@ -1782,7 +1984,7 @@
       <c r="AG11" s="9"/>
       <c r="AH11" s="2"/>
     </row>
-    <row r="12" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" ht="12.75">
       <c r="A12" s="6" t="s">
         <v>34</v>
       </c>
@@ -1848,7 +2050,9 @@
       <c r="Z12" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AA12" s="8"/>
+      <c r="AA12" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="AB12" s="10" t="s">
         <v>95</v>
       </c>
@@ -1861,7 +2065,7 @@
       <c r="AG12" s="9"/>
       <c r="AH12" s="2"/>
     </row>
-    <row r="13" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" ht="12.75">
       <c r="A13" s="6" t="s">
         <v>34</v>
       </c>
@@ -1942,7 +2146,7 @@
       <c r="AG13" s="9"/>
       <c r="AH13" s="2"/>
     </row>
-    <row r="14" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" ht="12.75">
       <c r="A14" s="6" t="s">
         <v>34</v>
       </c>
@@ -2021,7 +2225,7 @@
       <c r="AG14" s="9"/>
       <c r="AH14" s="2"/>
     </row>
-    <row r="15" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" ht="12.75">
       <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
@@ -2087,7 +2291,9 @@
       <c r="Z15" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AA15" s="8"/>
+      <c r="AA15" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="AB15" s="10" t="s">
         <v>95</v>
       </c>
@@ -2098,7 +2304,7 @@
       <c r="AG15" s="9"/>
       <c r="AH15" s="2"/>
     </row>
-    <row r="16" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34" ht="12.75">
       <c r="A16" s="6" t="s">
         <v>34</v>
       </c>
@@ -2177,7 +2383,7 @@
       <c r="AG16" s="9"/>
       <c r="AH16" s="2"/>
     </row>
-    <row r="17" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" ht="12.75">
       <c r="A17" s="6" t="s">
         <v>34</v>
       </c>
@@ -2256,7 +2462,7 @@
       <c r="AG17" s="9"/>
       <c r="AH17" s="2"/>
     </row>
-    <row r="18" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" ht="12.75">
       <c r="A18" s="6" t="s">
         <v>34</v>
       </c>
@@ -2335,7 +2541,7 @@
       <c r="AG18" s="9"/>
       <c r="AH18" s="2"/>
     </row>
-    <row r="19" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" ht="12.75">
       <c r="A19" s="8" t="s">
         <v>34</v>
       </c>
@@ -2416,7 +2622,7 @@
       <c r="AG19" s="9"/>
       <c r="AH19" s="3"/>
     </row>
-    <row r="20" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" ht="12.75">
       <c r="A20" s="8" t="s">
         <v>34</v>
       </c>
@@ -2497,7 +2703,7 @@
       <c r="AG20" s="9"/>
       <c r="AH20" s="3"/>
     </row>
-    <row r="21" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" ht="12.75">
       <c r="A21" s="8" t="s">
         <v>34</v>
       </c>
@@ -2578,7 +2784,7 @@
       <c r="AG21" s="9"/>
       <c r="AH21" s="3"/>
     </row>
-    <row r="22" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" ht="12.75">
       <c r="A22" s="8" t="s">
         <v>34</v>
       </c>
@@ -2659,7 +2865,7 @@
       <c r="AG22" s="9"/>
       <c r="AH22" s="3"/>
     </row>
-    <row r="23" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" ht="12.75">
       <c r="A23" s="8" t="s">
         <v>34</v>
       </c>
@@ -2740,7 +2946,7 @@
       <c r="AG23" s="9"/>
       <c r="AH23" s="3"/>
     </row>
-    <row r="24" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" ht="12.75">
       <c r="A24" s="8" t="s">
         <v>34</v>
       </c>
@@ -2821,7 +3027,7 @@
       <c r="AG24" s="9"/>
       <c r="AH24" s="3"/>
     </row>
-    <row r="25" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" ht="12.75">
       <c r="A25" s="8" t="s">
         <v>34</v>
       </c>
@@ -2889,7 +3095,9 @@
         <v>115</v>
       </c>
       <c r="Z25" s="9"/>
-      <c r="AA25" s="8"/>
+      <c r="AA25" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="AB25" s="9" t="s">
         <v>123</v>
       </c>
@@ -2900,7 +3108,7 @@
       <c r="AG25" s="9"/>
       <c r="AH25" s="3"/>
     </row>
-    <row r="26" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" ht="12.75">
       <c r="A26" s="8" t="s">
         <v>34</v>
       </c>
@@ -2981,7 +3189,7 @@
       <c r="AG26" s="9"/>
       <c r="AH26" s="3"/>
     </row>
-    <row r="27" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" ht="12.75">
       <c r="A27" s="8" t="s">
         <v>34</v>
       </c>
@@ -3062,7 +3270,7 @@
       <c r="AG27" s="9"/>
       <c r="AH27" s="3"/>
     </row>
-    <row r="28" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" ht="12.75">
       <c r="A28" s="8" t="s">
         <v>34</v>
       </c>
@@ -3143,7 +3351,7 @@
       <c r="AG28" s="9"/>
       <c r="AH28" s="3"/>
     </row>
-    <row r="29" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" ht="12.75">
       <c r="A29" s="8" t="s">
         <v>34</v>
       </c>
@@ -3224,7 +3432,7 @@
       <c r="AG29" s="9"/>
       <c r="AH29" s="3"/>
     </row>
-    <row r="30" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" ht="12.75">
       <c r="A30" s="8" t="s">
         <v>34</v>
       </c>
@@ -3305,7 +3513,7 @@
       <c r="AG30" s="9"/>
       <c r="AH30" s="3"/>
     </row>
-    <row r="31" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" ht="12.75">
       <c r="A31" s="8" t="s">
         <v>34</v>
       </c>
@@ -3386,7 +3594,7 @@
       <c r="AG31" s="9"/>
       <c r="AH31" s="3"/>
     </row>
-    <row r="32" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" ht="12.75">
       <c r="A32" s="8" t="s">
         <v>34</v>
       </c>
@@ -3467,7 +3675,7 @@
       <c r="AG32" s="9"/>
       <c r="AH32" s="3"/>
     </row>
-    <row r="33" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" ht="12.75">
       <c r="A33" s="8" t="s">
         <v>34</v>
       </c>
@@ -3535,7 +3743,9 @@
         <v>114</v>
       </c>
       <c r="Z33" s="8"/>
-      <c r="AA33" s="8"/>
+      <c r="AA33" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="AB33" s="9" t="s">
         <v>123</v>
       </c>
@@ -3548,7 +3758,7 @@
       <c r="AG33" s="9"/>
       <c r="AH33" s="3"/>
     </row>
-    <row r="34" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" ht="13.5" thickBot="1">
       <c r="A34" s="8" t="s">
         <v>34</v>
       </c>
@@ -3629,27 +3839,724 @@
       <c r="AG34" s="9"/>
       <c r="AH34" s="3"/>
     </row>
+    <row r="35" spans="1:34" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A35" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="17">
+        <v>2021</v>
+      </c>
+      <c r="C35" s="17">
+        <v>2</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H35" s="19"/>
+      <c r="I35" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="J35" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="N35" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="O35" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="P35" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q35" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="R35" s="19"/>
+      <c r="S35" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="T35" s="19"/>
+      <c r="U35" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="V35" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="W35" s="19"/>
+      <c r="X35" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y35" s="19"/>
+      <c r="Z35" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA35" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB35" s="19"/>
+      <c r="AC35" s="19"/>
+      <c r="AD35" s="19"/>
+      <c r="AE35" s="19"/>
+      <c r="AF35" s="19"/>
+      <c r="AG35" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="AH35" s="27"/>
+    </row>
+    <row r="36" spans="1:34" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A36" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="22">
+        <v>2021</v>
+      </c>
+      <c r="C36" s="22">
+        <v>2</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H36" s="24"/>
+      <c r="I36" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="J36" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="K36" s="24"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="N36" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="O36" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="P36" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q36" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="R36" s="24"/>
+      <c r="S36" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="T36" s="24"/>
+      <c r="U36" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="V36" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="W36" s="24"/>
+      <c r="X36" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y36" s="24"/>
+      <c r="Z36" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA36" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB36" s="24"/>
+      <c r="AC36" s="24"/>
+      <c r="AD36" s="24"/>
+      <c r="AE36" s="24"/>
+      <c r="AF36" s="24"/>
+      <c r="AG36" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="AH36" s="27"/>
+    </row>
+    <row r="37" spans="1:34" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A37" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="22">
+        <v>2021</v>
+      </c>
+      <c r="C37" s="22">
+        <v>2</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H37" s="24"/>
+      <c r="I37" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="J37" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="N37" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="O37" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="P37" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q37" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="R37" s="24"/>
+      <c r="S37" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="T37" s="24"/>
+      <c r="U37" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="V37" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="W37" s="24"/>
+      <c r="X37" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y37" s="24"/>
+      <c r="Z37" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA37" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB37" s="24"/>
+      <c r="AC37" s="24"/>
+      <c r="AD37" s="24"/>
+      <c r="AE37" s="24"/>
+      <c r="AF37" s="24"/>
+      <c r="AG37" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="AH37" s="27"/>
+    </row>
+    <row r="38" spans="1:34" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A38" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="22">
+        <v>2021</v>
+      </c>
+      <c r="C38" s="22">
+        <v>2</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H38" s="24"/>
+      <c r="I38" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="J38" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="K38" s="24"/>
+      <c r="L38" s="24"/>
+      <c r="M38" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="N38" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="O38" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="P38" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q38" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="R38" s="24"/>
+      <c r="S38" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="T38" s="24"/>
+      <c r="U38" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="V38" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="W38" s="24"/>
+      <c r="X38" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y38" s="24"/>
+      <c r="Z38" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA38" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB38" s="24"/>
+      <c r="AC38" s="24"/>
+      <c r="AD38" s="24"/>
+      <c r="AE38" s="24"/>
+      <c r="AF38" s="24"/>
+      <c r="AG38" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="AH38" s="27"/>
+    </row>
+    <row r="39" spans="1:34" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A39" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="22">
+        <v>2021</v>
+      </c>
+      <c r="C39" s="22">
+        <v>2</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H39" s="24"/>
+      <c r="I39" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="J39" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="K39" s="24"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="N39" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="O39" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="P39" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q39" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="R39" s="24"/>
+      <c r="S39" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="T39" s="24"/>
+      <c r="U39" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="V39" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="W39" s="24"/>
+      <c r="X39" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y39" s="24"/>
+      <c r="Z39" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA39" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB39" s="24"/>
+      <c r="AC39" s="24"/>
+      <c r="AD39" s="24"/>
+      <c r="AE39" s="24"/>
+      <c r="AF39" s="24"/>
+      <c r="AG39" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="AH39" s="27"/>
+    </row>
+    <row r="40" spans="1:34" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A40" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="22">
+        <v>2021</v>
+      </c>
+      <c r="C40" s="22">
+        <v>2</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G40" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H40" s="24"/>
+      <c r="I40" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="J40" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="K40" s="24"/>
+      <c r="L40" s="24"/>
+      <c r="M40" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="N40" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="O40" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="P40" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q40" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="R40" s="24"/>
+      <c r="S40" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="T40" s="24"/>
+      <c r="U40" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="V40" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="W40" s="24"/>
+      <c r="X40" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y40" s="24"/>
+      <c r="Z40" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA40" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB40" s="24"/>
+      <c r="AC40" s="24"/>
+      <c r="AD40" s="24"/>
+      <c r="AE40" s="24"/>
+      <c r="AF40" s="24"/>
+      <c r="AG40" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="AH40" s="27"/>
+    </row>
+    <row r="41" spans="1:34" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A41" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="22">
+        <v>2021</v>
+      </c>
+      <c r="C41" s="22">
+        <v>2</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G41" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H41" s="24"/>
+      <c r="I41" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="J41" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="K41" s="24"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="N41" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="O41" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="P41" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q41" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="R41" s="24"/>
+      <c r="S41" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="T41" s="24"/>
+      <c r="U41" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="V41" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="W41" s="24"/>
+      <c r="X41" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y41" s="24"/>
+      <c r="Z41" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA41" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB41" s="24"/>
+      <c r="AC41" s="24"/>
+      <c r="AD41" s="24"/>
+      <c r="AE41" s="24"/>
+      <c r="AF41" s="24"/>
+      <c r="AG41" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="AH41" s="27"/>
+    </row>
+    <row r="42" spans="1:34" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A42" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="22">
+        <v>2021</v>
+      </c>
+      <c r="C42" s="22">
+        <v>2</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F42" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G42" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H42" s="24"/>
+      <c r="I42" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="J42" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="K42" s="24"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="N42" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="O42" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="P42" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q42" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="R42" s="24"/>
+      <c r="S42" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="T42" s="24"/>
+      <c r="U42" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="V42" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="W42" s="24"/>
+      <c r="X42" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y42" s="24"/>
+      <c r="Z42" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA42" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB42" s="24"/>
+      <c r="AC42" s="24"/>
+      <c r="AD42" s="24"/>
+      <c r="AE42" s="24"/>
+      <c r="AF42" s="24"/>
+      <c r="AG42" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="AH42" s="27"/>
+    </row>
+    <row r="43" spans="1:34" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A43" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="22">
+        <v>2021</v>
+      </c>
+      <c r="C43" s="22">
+        <v>2</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G43" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H43" s="24"/>
+      <c r="I43" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="J43" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="K43" s="24"/>
+      <c r="L43" s="24"/>
+      <c r="M43" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="N43" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="O43" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="P43" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q43" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="R43" s="24"/>
+      <c r="S43" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="T43" s="24"/>
+      <c r="U43" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="V43" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="W43" s="24"/>
+      <c r="X43" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y43" s="24"/>
+      <c r="Z43" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA43" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB43" s="24"/>
+      <c r="AC43" s="24"/>
+      <c r="AD43" s="24"/>
+      <c r="AE43" s="24"/>
+      <c r="AF43" s="24"/>
+      <c r="AG43" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="AH43" s="27"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AH34" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH34">
-      <sortCondition sortBy="cellColor" ref="J1:J34" dxfId="0"/>
-    </sortState>
-  </autoFilter>
   <customSheetViews>
     <customSheetView guid="{D6C7FA59-6B7F-414D-B13B-8330DFCADBFC}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AG1656" xr:uid="{B9A58CA5-8FD8-44BB-8FBD-B0A7A3483740}"/>
+      <autoFilter ref="A1:AG1656"/>
     </customSheetView>
     <customSheetView guid="{61937B1B-5A62-4630-A349-DBF2AAB653FC}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AG1656" xr:uid="{1C644DA0-095C-48D0-9B29-E4A827520086}">
+      <autoFilter ref="A1:AG1656">
         <filterColumn colId="2">
-          <filters blank="1">
+          <filters>
             <filter val="2"/>
           </filters>
         </filterColumn>
         <filterColumn colId="3">
-          <filters blank="1">
+          <filters>
             <filter val="P"/>
           </filters>
         </filterColumn>
@@ -3662,7 +4569,7 @@
     </customSheetView>
     <customSheetView guid="{9504F232-F656-40EF-8B85-F2C095BEE71A}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AG930" xr:uid="{93079389-830F-4675-997C-BD27970AC2DE}">
+      <autoFilter ref="A1:AG930">
         <filterColumn colId="2">
           <filters>
             <filter val="6"/>
@@ -3685,7 +4592,7 @@
     </customSheetView>
     <customSheetView guid="{94EB77B4-A2D8-46C9-9348-39CA0F8EDAA6}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AG1656" xr:uid="{6370D338-2278-4393-B919-A5907E6C5D73}">
+      <autoFilter ref="A1:AG1656">
         <filterColumn colId="2">
           <filters blank="1">
             <filter val="2"/>
@@ -3701,7 +4608,7 @@
           </filters>
         </filterColumn>
         <filterColumn colId="20">
-          <filters blank="1">
+          <filters>
             <filter val="Categorico2"/>
           </filters>
         </filterColumn>
@@ -3709,15 +4616,15 @@
     </customSheetView>
     <customSheetView guid="{E02B9B3C-46F0-4728-91B3-E7CBF51265FB}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AH1655" xr:uid="{463CD196-8D0E-4B33-AAD0-23580570BFC3}"/>
+      <autoFilter ref="A1:AH1655"/>
     </customSheetView>
     <customSheetView guid="{FCCC49F7-5622-4BA0-827A-A37B5870D922}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AH1655" xr:uid="{A31FB958-4F4F-4BE2-8F2C-83F09B08FFA8}"/>
+      <autoFilter ref="A1:AH1655"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>